<commit_message>
actualizacion reporte de monitoreo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="1" state="visible" r:id="rId2"/>
@@ -255,7 +255,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -286,6 +286,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -452,16 +458,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -476,7 +486,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -485,10 +495,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,7 +522,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -556,11 +562,11 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -622,7 +628,7 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
@@ -640,7 +646,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -654,11 +660,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>totales</c:f>
+              <c:f>totales_planeados</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>totales</c:v>
+                  <c:v>totales_planeados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -730,11 +736,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>totales</c:f>
+              <c:f>totales_reales</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>totales</c:v>
+                  <c:v>totales_reales</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -804,152 +810,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>desviación</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>desviación</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Desviacion de esfuerzo'!$I$7:$I$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-9.09090909090909</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-15.0485436893204</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -959,16 +819,36 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="99861454"/>
-        <c:axId val="36416003"/>
+        <c:axId val="19253046"/>
+        <c:axId val="38989708"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99861454"/>
+        <c:axId val="19253046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Mes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -979,14 +859,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="36416003"/>
+        <c:crossAx val="38989708"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36416003"/>
+        <c:axId val="38989708"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1001,6 +881,26 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Tickets</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1011,7 +911,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99861454"/>
+        <c:crossAx val="19253046"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1046,7 +946,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1060,11 +960,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desviacion de costos'!$G$4</c:f>
+              <c:f>funcional</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Totales planeados</c:v>
+                  <c:v>funcional</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1085,291 +985,49 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Funcional!$D$4:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Entregables</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Control de cambios</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Línea base</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de costos'!$G$7:$G$18</c:f>
+              <c:f>Funcional!$D$17:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>140990.82</c:v>
+                  <c:v>83.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140990.82</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Desviacion de costos'!$H$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>totales Reales</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Desviacion de costos'!$H$7:$H$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>91828.107</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>81057.95</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>desviación</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>desviación</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>'Desviacion de costos'!$I$7:$I$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>-34.8694425637073</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-42.5083491251416</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="67848286"/>
-        <c:axId val="55311086"/>
+        <c:axId val="97132714"/>
+        <c:axId val="50136831"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="67848286"/>
+        <c:axId val="97132714"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1385,14 +1043,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55311086"/>
+        <c:crossAx val="50136831"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55311086"/>
+        <c:axId val="50136831"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1417,7 +1075,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="67848286"/>
+        <c:crossAx val="97132714"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1452,7 +1110,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1464,17 +1122,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>apego_interno</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>apego_interno</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="004586"/>
@@ -1493,41 +1140,198 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Apego a Procesos'!$D$4:$G$4</c:f>
+              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>Prospectación</c:v>
+                  <c:v>Enero</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Ventas</c:v>
+                  <c:v>Febrero</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Implementación</c:v>
+                  <c:v>Marzo</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Garantía</c:v>
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Apego a Procesos'!$D$17:$G$17</c:f>
+              <c:f>'Crecimiento anual de ventas'!$H$4:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>275000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>275000.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.57</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$J$4:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>179572.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134033.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1535,11 +1339,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="75458762"/>
-        <c:axId val="36378038"/>
+        <c:axId val="65310341"/>
+        <c:axId val="29368385"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75458762"/>
+        <c:axId val="65310341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1555,14 +1359,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="36378038"/>
+        <c:crossAx val="29368385"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36378038"/>
+        <c:axId val="29368385"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1587,7 +1391,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="75458762"/>
+        <c:crossAx val="65310341"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1622,7 +1426,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1636,11 +1440,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>procesos_organizacional</c:f>
+              <c:f>satisfacción</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>procesos_organizacional</c:v>
+                  <c:v>satisfacción</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1663,41 +1467,95 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Apego a Procesos'!$D$25:$G$25</c:f>
+              <c:f>'Indice de Satisfacción'!$C$5:$C$17</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>Calidad</c:v>
+                  <c:v>Enero</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Planeación anual</c:v>
+                  <c:v>Febrero</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Seguimiento</c:v>
+                  <c:v>Marzo</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Cambios</c:v>
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Apego a Procesos'!$D$38:$G$38</c:f>
+              <c:f>'Indice de Satisfacción'!$D$5:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>98.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>92.572</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95.686</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1705,11 +1563,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="4263083"/>
-        <c:axId val="30024363"/>
+        <c:axId val="86870159"/>
+        <c:axId val="52863315"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4263083"/>
+        <c:axId val="86870159"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,14 +1583,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="30024363"/>
+        <c:crossAx val="52863315"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30024363"/>
+        <c:axId val="52863315"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1615,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="4263083"/>
+        <c:crossAx val="86870159"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1792,7 +1650,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1806,11 +1664,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>proceso</c:f>
+              <c:f>desviación</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>proceso</c:v>
+                  <c:v>desviación</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1831,60 +1689,94 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Apego a Productos'!$D$4:$G$4</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Cotización</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Solicitud de compra</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Carta de aceptación</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Tickets de servicio</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Apego a Productos'!$D$17:$G$17</c:f>
+              <c:f>'Desviacion de esfuerzo'!$I$7:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>-9.09090909090909</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>-15.0485436893204</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>95</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="83657218"/>
-        <c:axId val="69645419"/>
+        <c:axId val="26322778"/>
+        <c:axId val="97593934"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83657218"/>
+        <c:axId val="26322778"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Mes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1895,14 +1787,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69645419"/>
+        <c:crossAx val="97593934"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69645419"/>
+        <c:axId val="97593934"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1917,6 +1809,26 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Porcentaje</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1927,7 +1839,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="83657218"/>
+        <c:crossAx val="26322778"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1962,7 +1874,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1976,11 +1888,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>organizacional</c:f>
+              <c:f>'Desviacion de costos'!$G$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>organizacional</c:v>
+                  <c:v>Totales planeados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2001,72 +1913,170 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Apego a Productos'!$D$26:$I$26</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>Catalogo de servicios</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Plan de calidad</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Plan de Métricas</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Plan de Configuración</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Plan de proyecto</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Reporte de Monitoreo</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Apego a Productos'!$D$39:$I$39</c:f>
+              <c:f>'Desviacion de costos'!$G$7:$G$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>140990.82</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>140990.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>88.9</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Desviacion de costos'!$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>totales Reales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Desviacion de costos'!$H$7:$H$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>91828.107</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>81057.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="13945438"/>
-        <c:axId val="35934031"/>
+        <c:axId val="66557972"/>
+        <c:axId val="3171250"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="13945438"/>
+        <c:axId val="66557972"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Mes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2077,14 +2087,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="35934031"/>
+        <c:crossAx val="3171250"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35934031"/>
+        <c:axId val="3171250"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,6 +2109,26 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Pesos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2109,7 +2139,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13945438"/>
+        <c:crossAx val="66557972"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2144,7 +2174,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2158,11 +2188,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>física</c:f>
+              <c:f>desviación</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>física</c:v>
+                  <c:v>desviación</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2183,60 +2213,94 @@
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
           </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Física!$D$6:$G$6</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Elementos de configuración física</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Control de cambios organizacional</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Línea base</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Elementos de Configuración</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Física!$D$19:$G$19</c:f>
+              <c:f>'Desviacion de costos'!$I$7:$I$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>-34.8694425637073</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>-42.5083491251416</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="33857728"/>
-        <c:axId val="8039124"/>
+        <c:axId val="8235349"/>
+        <c:axId val="45216745"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="33857728"/>
+        <c:axId val="8235349"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Mes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2247,14 +2311,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8039124"/>
+        <c:crossAx val="45216745"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8039124"/>
+        <c:axId val="45216745"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2269,6 +2333,26 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Porcentaje</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2279,7 +2363,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="33857728"/>
+        <c:crossAx val="8235349"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2314,7 +2398,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2328,11 +2412,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>funcional</c:f>
+              <c:f>apego_interno</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>funcional</c:v>
+                  <c:v>apego_interno</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2355,34 +2439,40 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Funcional!$D$4:$F$4</c:f>
+              <c:f>'Apego a Procesos'!$D$4:$G$4</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Entregables</c:v>
+                  <c:v>Prospectación</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Control de cambios</c:v>
+                  <c:v>Ventas</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Línea base</c:v>
+                  <c:v>Implementación</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Garantía</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Funcional!$D$17:$F$17</c:f>
+              <c:f>'Apego a Procesos'!$D$17:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>83.5</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>78.57</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -2391,11 +2481,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="39651859"/>
-        <c:axId val="2370812"/>
+        <c:axId val="18344368"/>
+        <c:axId val="34614624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39651859"/>
+        <c:axId val="18344368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2411,14 +2501,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="2370812"/>
+        <c:crossAx val="34614624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2370812"/>
+        <c:axId val="34614624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2443,7 +2533,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="39651859"/>
+        <c:crossAx val="18344368"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2478,7 +2568,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2490,6 +2580,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>procesos_organizacional</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>procesos_organizacional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:solidFill>
               <a:srgbClr val="004586"/>
@@ -2508,198 +2609,41 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
+              <c:f>'Apego a Procesos'!$D$25:$G$25</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Enero</c:v>
+                  <c:v>Calidad</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Febrero</c:v>
+                  <c:v>Planeación anual</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Marzo</c:v>
+                  <c:v>Seguimiento</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Abril</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mayo</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Junio</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Julio</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Agosto</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Septiembre</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Octubre</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Noviembre</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Diciembre</c:v>
+                  <c:v>Cambios</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Crecimiento anual de ventas'!$H$4:$H$15</c:f>
+              <c:f>'Apego a Procesos'!$D$38:$G$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>275000</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>275000.01</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Enero</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Febrero</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Marzo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Abril</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mayo</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Junio</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Julio</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Agosto</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Septiembre</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Octubre</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Noviembre</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Diciembre</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Crecimiento anual de ventas'!$J$4:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>179572.48</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>134033.44</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2707,11 +2651,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="68092718"/>
-        <c:axId val="69690542"/>
+        <c:axId val="78201251"/>
+        <c:axId val="43785690"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68092718"/>
+        <c:axId val="78201251"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2727,14 +2671,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69690542"/>
+        <c:crossAx val="43785690"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69690542"/>
+        <c:axId val="43785690"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2759,7 +2703,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68092718"/>
+        <c:crossAx val="78201251"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2794,7 +2738,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2808,11 +2752,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>satisfacción</c:f>
+              <c:f>proceso</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>satisfacción</c:v>
+                  <c:v>proceso</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2835,95 +2779,41 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Indice de Satisfacción'!$C$5:$C$17</c:f>
+              <c:f>'Apego a Productos'!$D$4:$G$4</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>Enero</c:v>
+                  <c:v>Cotización</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Febrero</c:v>
+                  <c:v>Solicitud de compra</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Marzo</c:v>
+                  <c:v>Carta de aceptación</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Abril</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mayo</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Junio</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Julio</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Agosto</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Septiembre</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Octubre</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Noviembre</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Diciembre</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Total</c:v>
+                  <c:v>Tickets de servicio</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Indice de Satisfacción'!$D$5:$D$17</c:f>
+              <c:f>'Apego a Productos'!$D$17:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>98.8</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>92.572</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>95.686</c:v>
+                  <c:v>95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2931,11 +2821,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="70252972"/>
-        <c:axId val="10969685"/>
+        <c:axId val="18264643"/>
+        <c:axId val="62816361"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70252972"/>
+        <c:axId val="18264643"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2951,14 +2841,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10969685"/>
+        <c:crossAx val="62816361"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10969685"/>
+        <c:axId val="62816361"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2983,7 +2873,359 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="70252972"/>
+        <c:crossAx val="18264643"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>organizacional</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>organizacional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Apego a Productos'!$D$26:$I$26</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Catalogo de servicios</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Plan de calidad</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Plan de Métricas</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Plan de Configuración</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Plan de proyecto</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Reporte de Monitoreo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Apego a Productos'!$D$39:$I$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="77506039"/>
+        <c:axId val="9764485"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="77506039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="9764485"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="9764485"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="77506039"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>física</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>física</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Física!$D$6:$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Elementos de configuración física</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Control de cambios organizacional</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Línea base</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Elementos de Configuración</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Física!$D$19:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="99162137"/>
+        <c:axId val="32461032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="99162137"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="32461032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="32461032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="99162137"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3023,15 +3265,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
+      <xdr:colOff>110520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>9720</xdr:rowOff>
+      <xdr:rowOff>13320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>81000</xdr:colOff>
+      <xdr:colOff>134280</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>15120</xdr:rowOff>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3039,12 +3281,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="259560" y="3744720"/>
-        <a:ext cx="5752800" cy="3243960"/>
+        <a:off x="313560" y="3726720"/>
+        <a:ext cx="5752080" cy="3243240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>529560</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>181440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>283320</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>186480</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6460920" y="3894840"/>
+        <a:ext cx="5755320" cy="3243600"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3058,28 +3330,58 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>220320</xdr:colOff>
+      <xdr:colOff>274320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>112320</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>83880</xdr:colOff>
+      <xdr:colOff>137160</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>91800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvPr id="2" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="423360" y="3664440"/>
-        <a:ext cx="5757480" cy="3236760"/>
+        <a:off x="477360" y="3646440"/>
+        <a:ext cx="5756760" cy="3236040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>624240</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>186120</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>425880</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>186840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="6721200" y="3738240"/>
+        <a:ext cx="5759280" cy="3239280"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3093,24 +3395,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>346680</xdr:colOff>
+      <xdr:colOff>400680</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1555560</xdr:colOff>
+      <xdr:colOff>1608840</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>151560</xdr:rowOff>
+      <xdr:rowOff>150840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Apego Interno"/>
+        <xdr:cNvPr id="4" name="Apego Interno"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8637120" y="0"/>
-        <a:ext cx="5756760" cy="3237480"/>
+        <a:off x="8691120" y="0"/>
+        <a:ext cx="5756040" cy="3236760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3123,24 +3425,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>463320</xdr:colOff>
+      <xdr:colOff>517320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>153720</xdr:rowOff>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1670040</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:colOff>1723320</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>185040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvPr id="5" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8753760" y="4001760"/>
-        <a:ext cx="5754600" cy="3229200"/>
+        <a:off x="8807760" y="3983760"/>
+        <a:ext cx="5753880" cy="3228480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3158,24 +3460,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>325800</xdr:colOff>
+      <xdr:colOff>379800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>156600</xdr:rowOff>
+      <xdr:rowOff>138600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>572400</xdr:colOff>
+      <xdr:colOff>625680</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvPr id="6" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8797320" y="156600"/>
-        <a:ext cx="5758200" cy="3236400"/>
+        <a:off x="8851320" y="138600"/>
+        <a:ext cx="5757480" cy="3235680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3188,24 +3490,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>356040</xdr:colOff>
+      <xdr:colOff>410040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>970920</xdr:colOff>
+      <xdr:colOff>1024200</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvPr id="7" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11253240" y="4310280"/>
-        <a:ext cx="5758200" cy="3234600"/>
+        <a:off x="11307240" y="4292280"/>
+        <a:ext cx="5757480" cy="3233880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3223,24 +3525,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>237960</xdr:colOff>
+      <xdr:colOff>291960</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>63720</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>407880</xdr:colOff>
+      <xdr:colOff>461160</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>114480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvPr id="8" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3794400" y="3578400"/>
-        <a:ext cx="5756040" cy="2995560"/>
+        <a:off x="3848400" y="3560400"/>
+        <a:ext cx="5755320" cy="2994840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3258,24 +3560,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>324360</xdr:colOff>
+      <xdr:colOff>378360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:rowOff>113400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>563400</xdr:colOff>
+      <xdr:colOff>616680</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvPr id="9" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7370280" y="131400"/>
-        <a:ext cx="5750640" cy="3233160"/>
+        <a:off x="7424280" y="113400"/>
+        <a:ext cx="5749920" cy="3232440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3293,24 +3595,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>158040</xdr:colOff>
+      <xdr:colOff>212040</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>5040</xdr:colOff>
+      <xdr:colOff>58320</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>42120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvPr id="10" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5718600" y="3137400"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="5772600" y="3119400"/>
+        <a:ext cx="5758200" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3328,24 +3630,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
+      <xdr:colOff>602640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:rowOff>106560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>137880</xdr:colOff>
+      <xdr:colOff>191160</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>141840</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvPr id="11" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4052520" y="665280"/>
-        <a:ext cx="5761440" cy="3233160"/>
+        <a:off x="4106520" y="647280"/>
+        <a:ext cx="5760720" cy="3232440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3363,10 +3665,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:I65536"/>
+  <dimension ref="B1:K65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3554,7 +3856,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
@@ -3575,7 +3877,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
@@ -3595,6 +3897,7 @@
         <f aca="false">((H12 * 100)/G12)-100</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
@@ -3815,8 +4118,8 @@
   </sheetPr>
   <dimension ref="B1:K65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K17" activeCellId="0" sqref="K17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F36" activeCellId="0" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3918,34 +4221,34 @@
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11" t="n">
+      <c r="C7" s="12" t="n">
         <v>63870.88</v>
       </c>
-      <c r="D7" s="11" t="n">
+      <c r="D7" s="12" t="n">
         <v>57896.127</v>
       </c>
-      <c r="E7" s="11" t="n">
+      <c r="E7" s="12" t="n">
         <v>77119.94</v>
       </c>
-      <c r="F7" s="11" t="n">
+      <c r="F7" s="12" t="n">
         <v>33931.98</v>
       </c>
-      <c r="G7" s="12" t="n">
+      <c r="G7" s="13" t="n">
         <f aca="false">SUM(C7,E7)</f>
         <v>140990.82</v>
       </c>
-      <c r="H7" s="13" t="n">
+      <c r="H7" s="14" t="n">
         <f aca="false">SUM(D7,F7)</f>
         <v>91828.107</v>
       </c>
-      <c r="I7" s="14" t="n">
+      <c r="I7" s="15" t="n">
         <f aca="false">((H7 * 100)/G7)-100</f>
         <v>-34.8694425637073</v>
       </c>
-      <c r="J7" s="15" t="n">
+      <c r="J7" s="16" t="n">
         <v>88924.64</v>
       </c>
-      <c r="K7" s="13" t="n">
+      <c r="K7" s="14" t="n">
         <f aca="false">SUM(J7,H7)</f>
         <v>180752.747</v>
       </c>
@@ -3954,34 +4257,34 @@
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="11" t="n">
+      <c r="C8" s="12" t="n">
         <v>63870.88</v>
       </c>
-      <c r="D8" s="11" t="n">
+      <c r="D8" s="12" t="n">
         <v>60118.7</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="E8" s="12" t="n">
         <v>77119.94</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="12" t="n">
         <v>20939.25</v>
       </c>
-      <c r="G8" s="12" t="n">
+      <c r="G8" s="13" t="n">
         <f aca="false">SUM(C8,E8)</f>
         <v>140990.82</v>
       </c>
-      <c r="H8" s="13" t="n">
+      <c r="H8" s="14" t="n">
         <f aca="false">SUM(D8,F8)</f>
         <v>81057.95</v>
       </c>
-      <c r="I8" s="16" t="n">
+      <c r="I8" s="17" t="n">
         <f aca="false">((H8 * 100)/G8)-100</f>
         <v>-42.5083491251416</v>
       </c>
-      <c r="J8" s="15" t="n">
+      <c r="J8" s="16" t="n">
         <v>60762.1</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="K8" s="14" t="n">
         <f aca="false">SUM(J8,H8)</f>
         <v>141820.05</v>
       </c>
@@ -3990,231 +4293,231 @@
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12" t="n">
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13" t="n">
         <f aca="false">SUM(C9,E9)</f>
         <v>0</v>
       </c>
-      <c r="H9" s="13" t="n">
+      <c r="H9" s="14" t="n">
         <f aca="false">SUM(D9,F9)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="17" t="e">
+      <c r="I9" s="10" t="e">
         <f aca="false">((H9 * 100)/G9)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J9" s="11"/>
-      <c r="K9" s="13"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12" t="n">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13" t="n">
         <f aca="false">SUM(C10,E10)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="13" t="n">
+      <c r="H10" s="14" t="n">
         <f aca="false">SUM(D10,F10)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="17" t="e">
+      <c r="I10" s="10" t="e">
         <f aca="false">((H10 * 100)/G10)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="13"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="12" t="n">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13" t="n">
         <f aca="false">SUM(C11,E11)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="13" t="n">
+      <c r="H11" s="14" t="n">
         <f aca="false">SUM(D11,F11)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="17" t="e">
+      <c r="I11" s="10" t="e">
         <f aca="false">((H11 * 100)/G11)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="13"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="12" t="n">
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13" t="n">
         <f aca="false">SUM(C12,E12)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="13" t="n">
+      <c r="H12" s="14" t="n">
         <f aca="false">SUM(D12,F12)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="17" t="e">
+      <c r="I12" s="10" t="e">
         <f aca="false">((H12 * 100)/G12)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J12" s="11"/>
-      <c r="K12" s="13"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="12" t="n">
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13" t="n">
         <f aca="false">SUM(C13,E13)</f>
         <v>0</v>
       </c>
-      <c r="H13" s="13" t="n">
+      <c r="H13" s="14" t="n">
         <f aca="false">SUM(D13,F13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="17" t="e">
+      <c r="I13" s="10" t="e">
         <f aca="false">((H13 * 100)/G13)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="13"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="12" t="n">
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13" t="n">
         <f aca="false">SUM(C14,E14)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="13" t="n">
+      <c r="H14" s="14" t="n">
         <f aca="false">SUM(D14,F14)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="17" t="e">
+      <c r="I14" s="10" t="e">
         <f aca="false">((H14 * 100)/G14)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J14" s="11"/>
-      <c r="K14" s="13"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="12" t="n">
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="13" t="n">
         <f aca="false">SUM(C15,E15)</f>
         <v>0</v>
       </c>
-      <c r="H15" s="13" t="n">
+      <c r="H15" s="14" t="n">
         <f aca="false">SUM(D15,F15)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="17" t="e">
+      <c r="I15" s="10" t="e">
         <f aca="false">((H15 * 100)/G15)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J15" s="11"/>
-      <c r="K15" s="13"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="14"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="12" t="n">
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="13" t="n">
         <f aca="false">SUM(C16,E16)</f>
         <v>0</v>
       </c>
-      <c r="H16" s="13" t="n">
+      <c r="H16" s="14" t="n">
         <f aca="false">SUM(D16,F16)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="17" t="e">
+      <c r="I16" s="10" t="e">
         <f aca="false">((H16 * 100)/G16)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="13"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="14"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="12" t="n">
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13" t="n">
         <f aca="false">SUM(C17,E17)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="13" t="n">
+      <c r="H17" s="14" t="n">
         <f aca="false">SUM(D17,F17)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="17" t="e">
+      <c r="I17" s="10" t="e">
         <f aca="false">((H17 * 100)/G17)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="13"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="12" t="n">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13" t="n">
         <f aca="false">SUM(C18,E18)</f>
         <v>0</v>
       </c>
-      <c r="H18" s="13" t="n">
+      <c r="H18" s="14" t="n">
         <f aca="false">SUM(D18,F18)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="17" t="e">
+      <c r="I18" s="10" t="e">
         <f aca="false">((H18 * 100)/G18)-100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="13"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="14"/>
     </row>
     <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -4274,8 +4577,8 @@
   </sheetPr>
   <dimension ref="C1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5693,31 +5996,31 @@
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="13" t="n">
+      <c r="B4" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="13" t="n">
+      <c r="C4" s="14" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="14" t="n">
         <f aca="false">275000/2</f>
         <v>137500</v>
       </c>
-      <c r="E4" s="13" t="n">
+      <c r="E4" s="14" t="n">
         <v>26640.42</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="14" t="n">
         <f aca="false">275000/2</f>
         <v>137500</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="14" t="n">
         <v>18065.18</v>
       </c>
       <c r="H4" s="32" t="n">
         <f aca="false">SUM(B4,F4,D4)</f>
         <v>275000</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I4" s="14" t="n">
         <f aca="false">SUM(C4,G4,E4)</f>
         <v>44705.6</v>
       </c>
@@ -5737,29 +6040,29 @@
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="13" t="n">
+      <c r="B5" s="14" t="n">
         <v>91666.67</v>
       </c>
-      <c r="C5" s="13" t="n">
+      <c r="C5" s="14" t="n">
         <v>11997</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="14" t="n">
         <v>91666.67</v>
       </c>
-      <c r="E5" s="13" t="n">
+      <c r="E5" s="14" t="n">
         <v>12722.43</v>
       </c>
-      <c r="F5" s="13" t="n">
+      <c r="F5" s="14" t="n">
         <v>91666.67</v>
       </c>
-      <c r="G5" s="13" t="n">
+      <c r="G5" s="14" t="n">
         <v>25179.75</v>
       </c>
       <c r="H5" s="32" t="n">
         <f aca="false">SUM(B5,F5,D5)</f>
         <v>275000.01</v>
       </c>
-      <c r="I5" s="13" t="n">
+      <c r="I5" s="14" t="n">
         <f aca="false">SUM(C5,G5,E5)</f>
         <v>49899.18</v>
       </c>
@@ -5779,17 +6082,17 @@
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="32" t="n">
         <f aca="false">SUM(B6,F6,D6)</f>
         <v>0</v>
       </c>
-      <c r="I6" s="13" t="n">
+      <c r="I6" s="14" t="n">
         <f aca="false">SUM(C6,G6,E6)</f>
         <v>0</v>
       </c>
@@ -5804,17 +6107,17 @@
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="32" t="n">
         <f aca="false">SUM(B7,F7,D7)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="13" t="n">
+      <c r="I7" s="14" t="n">
         <f aca="false">SUM(C7,G7,E7)</f>
         <v>0</v>
       </c>
@@ -5829,17 +6132,17 @@
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="32" t="n">
         <f aca="false">SUM(B8,F8,D8)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="13" t="n">
+      <c r="I8" s="14" t="n">
         <f aca="false">SUM(C8,G8,E8)</f>
         <v>0</v>
       </c>
@@ -5854,17 +6157,17 @@
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="32" t="n">
         <f aca="false">SUM(B9,F9,D9)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="13" t="n">
+      <c r="I9" s="14" t="n">
         <f aca="false">SUM(C9,G9,E9)</f>
         <v>0</v>
       </c>
@@ -5879,17 +6182,17 @@
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="32" t="n">
         <f aca="false">SUM(B10,F10,D10)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="13" t="n">
+      <c r="I10" s="14" t="n">
         <f aca="false">SUM(C10,G10,E10)</f>
         <v>0</v>
       </c>
@@ -5904,17 +6207,17 @@
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="32" t="n">
         <f aca="false">SUM(B11,F11,D11)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="13" t="n">
+      <c r="I11" s="14" t="n">
         <f aca="false">SUM(C11,G11,E11)</f>
         <v>0</v>
       </c>
@@ -5929,17 +6232,17 @@
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="32" t="n">
         <f aca="false">SUM(B12,F12,D12)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="13" t="n">
+      <c r="I12" s="14" t="n">
         <f aca="false">SUM(C12,G12,E12)</f>
         <v>0</v>
       </c>
@@ -5954,17 +6257,17 @@
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="32" t="n">
         <f aca="false">SUM(B13,F13,D13)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="13" t="n">
+      <c r="I13" s="14" t="n">
         <f aca="false">SUM(C13,G13,E13)</f>
         <v>0</v>
       </c>
@@ -5979,17 +6282,17 @@
       <c r="A14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="32" t="n">
         <f aca="false">SUM(B14,F14,D14)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="13" t="n">
+      <c r="I14" s="14" t="n">
         <f aca="false">SUM(C14,G14,E14)</f>
         <v>0</v>
       </c>
@@ -6004,17 +6307,17 @@
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="32" t="n">
         <f aca="false">SUM(B15,F15,D15)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="13" t="n">
+      <c r="I15" s="14" t="n">
         <f aca="false">SUM(C15,G15,E15)</f>
         <v>0</v>
       </c>
@@ -6029,27 +6332,27 @@
       <c r="A16" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="13" t="n">
+      <c r="B16" s="14" t="n">
         <f aca="false">SUM(B4:B15)</f>
         <v>91666.67</v>
       </c>
-      <c r="C16" s="13" t="n">
+      <c r="C16" s="14" t="n">
         <f aca="false">SUM(C4:C15)</f>
         <v>11997</v>
       </c>
-      <c r="D16" s="13" t="n">
+      <c r="D16" s="14" t="n">
         <f aca="false">SUM(D4:D15)</f>
         <v>229166.67</v>
       </c>
-      <c r="E16" s="13" t="n">
+      <c r="E16" s="14" t="n">
         <f aca="false">SUM(E4:E15)</f>
         <v>39362.85</v>
       </c>
-      <c r="F16" s="13" t="n">
+      <c r="F16" s="14" t="n">
         <f aca="false">SUM(F4:F15)</f>
         <v>229166.67</v>
       </c>
-      <c r="G16" s="13" t="n">
+      <c r="G16" s="14" t="n">
         <f aca="false">SUM(G4:G15)</f>
         <v>43244.93</v>
       </c>
@@ -6057,7 +6360,7 @@
         <f aca="false">SUM(H4:H15)</f>
         <v>550000.01</v>
       </c>
-      <c r="I16" s="13" t="n">
+      <c r="I16" s="14" t="n">
         <f aca="false">SUM(I4:I15)</f>
         <v>94604.78</v>
       </c>
@@ -6085,7 +6388,7 @@
       <c r="B20" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="C20" s="13" t="n">
+      <c r="C20" s="14" t="n">
         <v>3300000</v>
       </c>
     </row>
@@ -6093,7 +6396,7 @@
       <c r="B21" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="13" t="n">
+      <c r="C21" s="14" t="n">
         <f aca="false">J16</f>
         <v>313605.92</v>
       </c>
@@ -6139,7 +6442,7 @@
   </sheetPr>
   <dimension ref="C2:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Actualización de plantillas organizacionales, plan de métricas y linea base
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
@@ -16,13 +16,15 @@
     <sheet name="Funcional" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="Crecimiento anual de ventas" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Indice de Satisfacción" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="Producto" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="Actividades" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="79">
   <si>
     <t>Desviación de esfuerzo por proyectos planificados/reales</t>
   </si>
@@ -244,6 +246,21 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>abril</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Actividades en tiempo</t>
+  </si>
+  <si>
+    <t>Actividades fuera de tiempo</t>
   </si>
 </sst>
 </file>
@@ -255,7 +272,7 @@
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -285,6 +302,11 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -301,6 +323,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -425,7 +452,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -486,7 +513,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -522,7 +549,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -562,16 +589,28 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -646,10 +685,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Esfuerzo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -817,13 +876,23 @@
             </a:ln>
           </c:spPr>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="19253046"/>
-        <c:axId val="38989708"/>
+        <c:axId val="96814414"/>
+        <c:axId val="46892396"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="19253046"/>
+        <c:axId val="96814414"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -859,14 +928,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="38989708"/>
+        <c:crossAx val="46892396"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38989708"/>
+        <c:axId val="46892396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +980,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19253046"/>
+        <c:crossAx val="96814414"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -946,714 +1015,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:plotArea>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Desviación de Esfuerzo</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>funcional</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>funcional</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Funcional!$D$4:$F$4</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Entregables</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Control de cambios</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Línea base</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Funcional!$D$17:$F$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>83.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="97132714"/>
-        <c:axId val="50136831"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="97132714"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="50136831"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50136831"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="97132714"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Enero</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Febrero</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Marzo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Abril</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mayo</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Junio</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Julio</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Agosto</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Septiembre</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Octubre</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Noviembre</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Diciembre</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Crecimiento anual de ventas'!$H$4:$H$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>275000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>275000.01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>Enero</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Febrero</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Marzo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Abril</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mayo</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Junio</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Julio</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Agosto</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Septiembre</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Octubre</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Noviembre</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Diciembre</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Crecimiento anual de ventas'!$J$4:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>179572.48</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>134033.44</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="65310341"/>
-        <c:axId val="29368385"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="65310341"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="29368385"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="29368385"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="65310341"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>satisfacción</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>satisfacción</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Indice de Satisfacción'!$C$5:$C$17</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>Enero</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Febrero</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Marzo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Abril</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mayo</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Junio</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Julio</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Agosto</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Septiembre</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Octubre</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Noviembre</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Diciembre</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Indice de Satisfacción'!$D$5:$D$17</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>98.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>92.572</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>95.686</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="86870159"/>
-        <c:axId val="52863315"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="86870159"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="52863315"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="52863315"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="86870159"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -1745,13 +1130,23 @@
             </a:ln>
           </c:spPr>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="26322778"/>
-        <c:axId val="97593934"/>
+        <c:axId val="28105241"/>
+        <c:axId val="56153898"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="26322778"/>
+        <c:axId val="28105241"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1787,14 +1182,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="97593934"/>
+        <c:crossAx val="56153898"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97593934"/>
+        <c:axId val="56153898"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1839,7 +1234,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26322778"/>
+        <c:crossAx val="28105241"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1874,10 +1269,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart69.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Costos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2045,13 +1460,23 @@
             </a:ln>
           </c:spPr>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="66557972"/>
-        <c:axId val="3171250"/>
+        <c:axId val="61155153"/>
+        <c:axId val="83023922"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="66557972"/>
+        <c:axId val="61155153"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2087,14 +1512,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3171250"/>
+        <c:crossAx val="83023922"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3171250"/>
+        <c:axId val="83023922"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2139,7 +1564,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="66557972"/>
+        <c:crossAx val="61155153"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2174,10 +1599,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart70.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Desviación de costos</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2269,13 +1714,23 @@
             </a:ln>
           </c:spPr>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="8235349"/>
-        <c:axId val="45216745"/>
+        <c:axId val="5971967"/>
+        <c:axId val="34751603"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="8235349"/>
+        <c:axId val="5971967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2311,14 +1766,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45216745"/>
+        <c:crossAx val="34751603"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45216745"/>
+        <c:axId val="34751603"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2363,7 +1818,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8235349"/>
+        <c:crossAx val="5971967"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2398,10 +1853,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart71.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Apego a productos proceso</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2481,11 +1956,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="18344368"/>
-        <c:axId val="34614624"/>
+        <c:axId val="7155355"/>
+        <c:axId val="83148861"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18344368"/>
+        <c:axId val="7155355"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2501,14 +1976,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="34614624"/>
+        <c:crossAx val="83148861"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34614624"/>
+        <c:axId val="83148861"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2533,7 +2008,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18344368"/>
+        <c:crossAx val="7155355"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2568,10 +2043,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart72.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Apego a procesos organizacionales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2651,11 +2146,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="78201251"/>
-        <c:axId val="43785690"/>
+        <c:axId val="79535569"/>
+        <c:axId val="51999893"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78201251"/>
+        <c:axId val="79535569"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2671,14 +2166,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="43785690"/>
+        <c:crossAx val="51999893"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43785690"/>
+        <c:axId val="51999893"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2703,7 +2198,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="78201251"/>
+        <c:crossAx val="79535569"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2738,10 +2233,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart73.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Apego a productos entrega de servicio</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2821,11 +2336,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="18264643"/>
-        <c:axId val="62816361"/>
+        <c:axId val="43833675"/>
+        <c:axId val="59788129"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="18264643"/>
+        <c:axId val="43833675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2841,14 +2356,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="62816361"/>
+        <c:crossAx val="59788129"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62816361"/>
+        <c:axId val="59788129"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2873,7 +2388,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18264643"/>
+        <c:crossAx val="43833675"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2908,10 +2423,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart74.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Auditoria productos organizacionales</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3003,11 +2538,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="77506039"/>
-        <c:axId val="9764485"/>
+        <c:axId val="88689457"/>
+        <c:axId val="90490595"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77506039"/>
+        <c:axId val="88689457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3023,14 +2558,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="9764485"/>
+        <c:crossAx val="90490595"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9764485"/>
+        <c:axId val="90490595"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3055,7 +2590,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77506039"/>
+        <c:crossAx val="88689457"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3090,10 +2625,30 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart75.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Auditoría Física</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -3173,11 +2728,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="99162137"/>
-        <c:axId val="32461032"/>
+        <c:axId val="23652454"/>
+        <c:axId val="91927656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99162137"/>
+        <c:axId val="23652454"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3193,14 +2748,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="32461032"/>
+        <c:crossAx val="91927656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="32461032"/>
+        <c:axId val="91927656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3225,7 +2780,962 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99162137"/>
+        <c:crossAx val="23652454"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart76.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Auditoría funcional</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>funcional</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>funcional</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Funcional!$D$4:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Entregables</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Control de cambios</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Línea base</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Funcional!$D$17:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>83.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="3697499"/>
+        <c:axId val="5485395"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="3697499"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="5485395"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="5485395"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="3697499"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart77.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Crecimiento anual de ventas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$H$4:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>275000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>275000.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Crecimiento anual de ventas'!$A$4:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Crecimiento anual de ventas'!$J$4:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>179572.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134033.44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="60807637"/>
+        <c:axId val="24844309"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="60807637"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="24844309"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="24844309"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="60807637"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Indice de satisfacció n</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>satisfacción</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>satisfacción</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Indice de Satisfacción'!$C$5:$C$17</c:f>
+              <c:strCache>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Julio</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Agosto</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Septiembre</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Octubre</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Noviembre</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Diciembre</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Indice de Satisfacción'!$D$5:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>98.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>92.572</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>95.686</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="61791844"/>
+        <c:axId val="87188256"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="61791844"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="87188256"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="87188256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="61791844"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart79.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Grafico de actividades</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Actividades!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Actividades!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Porcentaje</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Actividades!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="2810488"/>
+        <c:axId val="51014468"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2810488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="51014468"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51014468"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Porcentaje</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="2810488"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3265,15 +3775,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>110520</xdr:colOff>
+      <xdr:colOff>137520</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>4320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>134280</xdr:colOff>
+      <xdr:colOff>160920</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3281,8 +3791,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="313560" y="3726720"/>
-        <a:ext cx="5752080" cy="3243240"/>
+        <a:off x="340560" y="3717720"/>
+        <a:ext cx="5751720" cy="3242880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3295,15 +3805,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>529560</xdr:colOff>
+      <xdr:colOff>556560</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>181440</xdr:rowOff>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>283320</xdr:colOff>
+      <xdr:colOff>309960</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>186480</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3311,8 +3821,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6460920" y="3894840"/>
-        <a:ext cx="5755320" cy="3243600"/>
+        <a:off x="6487920" y="3885840"/>
+        <a:ext cx="5754960" cy="3243240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3330,15 +3840,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
+      <xdr:colOff>301320</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>94320</xdr:rowOff>
+      <xdr:rowOff>85320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
+      <xdr:colOff>163800</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:rowOff>82440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3346,8 +3856,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="477360" y="3646440"/>
-        <a:ext cx="5756760" cy="3236040"/>
+        <a:off x="504360" y="3637440"/>
+        <a:ext cx="5756400" cy="3235680"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3360,15 +3870,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>624240</xdr:colOff>
+      <xdr:colOff>651240</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>186120</xdr:rowOff>
+      <xdr:rowOff>177120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>425880</xdr:colOff>
+      <xdr:colOff>452520</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>186840</xdr:rowOff>
+      <xdr:rowOff>177480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3376,8 +3886,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6721200" y="3738240"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:off x="6748200" y="3729240"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3395,15 +3905,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>400680</xdr:colOff>
+      <xdr:colOff>427680</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1608840</xdr:colOff>
+      <xdr:colOff>1635480</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>150840</xdr:rowOff>
+      <xdr:rowOff>150480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3411,8 +3921,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8691120" y="0"/>
-        <a:ext cx="5756040" cy="3236760"/>
+        <a:off x="8718120" y="0"/>
+        <a:ext cx="5755680" cy="3236400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3425,15 +3935,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>517320</xdr:colOff>
+      <xdr:colOff>544320</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1723320</xdr:colOff>
+      <xdr:colOff>1749960</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>185040</xdr:rowOff>
+      <xdr:rowOff>175680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3441,8 +3951,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8807760" y="3983760"/>
-        <a:ext cx="5753880" cy="3228480"/>
+        <a:off x="8834760" y="3974760"/>
+        <a:ext cx="5753520" cy="3228120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3460,15 +3970,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>379800</xdr:colOff>
+      <xdr:colOff>406800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>138600</xdr:rowOff>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>625680</xdr:colOff>
+      <xdr:colOff>652320</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3476,8 +3986,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8851320" y="138600"/>
-        <a:ext cx="5757480" cy="3235680"/>
+        <a:off x="8878320" y="129600"/>
+        <a:ext cx="5757120" cy="3235320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3490,15 +4000,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>410040</xdr:colOff>
+      <xdr:colOff>437040</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>1024200</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>21960</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3506,8 +4016,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11307240" y="4292280"/>
-        <a:ext cx="5757480" cy="3233880"/>
+        <a:off x="11334240" y="4283280"/>
+        <a:ext cx="5757120" cy="3233520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3524,16 +4034,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>865080</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>15120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>461160</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>623160</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>83520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3541,8 +4051,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3848400" y="3560400"/>
-        <a:ext cx="5755320" cy="2994840"/>
+        <a:off x="6068160" y="4505040"/>
+        <a:ext cx="5754960" cy="2994480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3560,15 +4070,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>378360</xdr:colOff>
+      <xdr:colOff>405360</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>616680</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:colOff>643320</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>172440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3576,8 +4086,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7424280" y="113400"/>
-        <a:ext cx="5749920" cy="3232440"/>
+        <a:off x="7451280" y="104400"/>
+        <a:ext cx="5749560" cy="3232080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3595,15 +4105,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>212040</xdr:colOff>
+      <xdr:colOff>239040</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>124920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>58320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>42120</xdr:rowOff>
+      <xdr:rowOff>32760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3611,8 +4121,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5772600" y="3119400"/>
-        <a:ext cx="5758200" cy="3238200"/>
+        <a:off x="5799600" y="3110400"/>
+        <a:ext cx="5757840" cy="3237840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3630,15 +4140,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>602640</xdr:colOff>
+      <xdr:colOff>629640</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>106560</xdr:rowOff>
+      <xdr:rowOff>97560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>191160</xdr:colOff>
+      <xdr:colOff>217800</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>113760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3646,8 +4156,43 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4106520" y="647280"/>
-        <a:ext cx="5760720" cy="3232440"/>
+        <a:off x="4133520" y="638280"/>
+        <a:ext cx="5760360" cy="3232080"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>487800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>32760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>557640</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>108360</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5627880" y="32760"/>
+        <a:ext cx="5759640" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3668,7 +4213,7 @@
   <dimension ref="B1:K65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D38" activeCellId="0" sqref="D38"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4111,6 +4656,184 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.6113360323887"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8623481781377"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6396761133603"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="39" t="e">
+        <f aca="false">C2/SUM(C2:D2)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="39" t="e">
+        <f aca="false">C3/SUM(C3:D3)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="39" t="e">
+        <f aca="false">C4/SUM(C4:D4)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="39" t="e">
+        <f aca="false">C5/SUM(C5:D5)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="39" t="e">
+        <f aca="false">C6/SUM(C6:D6)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="39" t="e">
+        <f aca="false">C7/SUM(C7:D7)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="39" t="e">
+        <f aca="false">C8/SUM(C8:D8)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="39" t="e">
+        <f aca="false">C9/SUM(C9:D9)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="39" t="e">
+        <f aca="false">C10/SUM(C10:D10)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="39" t="e">
+        <f aca="false">C11/SUM(C11:D11)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="39" t="e">
+        <f aca="false">C12/SUM(C12:D12)*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="39" t="e">
+        <f aca="false">C13/SUM(C13:D13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -4577,8 +5300,8 @@
   </sheetPr>
   <dimension ref="C1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5003,8 +5726,8 @@
   </sheetPr>
   <dimension ref="C1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M22" activeCellId="0" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5477,8 +6200,8 @@
   </sheetPr>
   <dimension ref="C1:G19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6442,8 +7165,8 @@
   </sheetPr>
   <dimension ref="C2:D65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6578,4 +7301,141 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8097165991903"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="18.9878542510121"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Concentrado de Métricas actualziacion marzo
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Desviacion de esfuerzo" sheetId="1" state="visible" r:id="rId2"/>
@@ -837,7 +837,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart71.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1106,11 +1106,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="52587386"/>
-        <c:axId val="55192635"/>
+        <c:axId val="83608227"/>
+        <c:axId val="70359509"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52587386"/>
+        <c:axId val="83608227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,14 +1126,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="55192635"/>
+        <c:crossAx val="70359509"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55192635"/>
+        <c:axId val="70359509"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1158,7 +1158,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="52587386"/>
+        <c:crossAx val="83608227"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1193,7 +1193,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart72.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1462,11 +1462,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="51495926"/>
-        <c:axId val="28433031"/>
+        <c:axId val="63813599"/>
+        <c:axId val="22954217"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51495926"/>
+        <c:axId val="63813599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1482,14 +1482,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="28433031"/>
+        <c:crossAx val="22954217"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="28433031"/>
+        <c:axId val="22954217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1514,7 +1514,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51495926"/>
+        <c:crossAx val="63813599"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1549,7 +1549,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart73.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1699,11 +1699,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="57964230"/>
-        <c:axId val="89995083"/>
+        <c:axId val="73814135"/>
+        <c:axId val="99773105"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57964230"/>
+        <c:axId val="73814135"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1719,14 +1719,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89995083"/>
+        <c:crossAx val="99773105"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89995083"/>
+        <c:axId val="99773105"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1751,7 +1751,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="57964230"/>
+        <c:crossAx val="73814135"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1786,7 +1786,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart74.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1936,11 +1936,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="91942258"/>
-        <c:axId val="96353394"/>
+        <c:axId val="31027127"/>
+        <c:axId val="31609572"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="91942258"/>
+        <c:axId val="31027127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1956,14 +1956,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96353394"/>
+        <c:crossAx val="31609572"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96353394"/>
+        <c:axId val="31609572"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1988,7 +1988,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="91942258"/>
+        <c:crossAx val="31027127"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2023,7 +2023,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart75.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2274,11 +2274,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="77904198"/>
-        <c:axId val="27294192"/>
+        <c:axId val="31235635"/>
+        <c:axId val="90843795"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77904198"/>
+        <c:axId val="31235635"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,14 +2295,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27294192"/>
+        <c:crossAx val="90843795"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="27294192"/>
+        <c:axId val="90843795"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2326,7 +2326,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77904198"/>
+        <c:crossAx val="31235635"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2362,7 +2362,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart76.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2482,11 +2482,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="84975712"/>
-        <c:axId val="64708621"/>
+        <c:axId val="1037796"/>
+        <c:axId val="64969534"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="84975712"/>
+        <c:axId val="1037796"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2503,14 +2503,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="64708621"/>
+        <c:crossAx val="64969534"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64708621"/>
+        <c:axId val="64969534"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2534,7 +2534,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84975712"/>
+        <c:crossAx val="1037796"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2560,7 +2560,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart77.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2642,11 +2642,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="22472729"/>
-        <c:axId val="92153817"/>
+        <c:axId val="90178700"/>
+        <c:axId val="29711994"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="22472729"/>
+        <c:axId val="90178700"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2662,14 +2662,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92153817"/>
+        <c:crossAx val="29711994"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92153817"/>
+        <c:axId val="29711994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2694,7 +2694,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="22472729"/>
+        <c:crossAx val="90178700"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2729,7 +2729,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart78.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2800,11 +2800,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="51137712"/>
-        <c:axId val="19950501"/>
+        <c:axId val="55247589"/>
+        <c:axId val="49895277"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51137712"/>
+        <c:axId val="55247589"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2820,14 +2820,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19950501"/>
+        <c:crossAx val="49895277"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19950501"/>
+        <c:axId val="49895277"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2852,7 +2852,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="51137712"/>
+        <c:crossAx val="55247589"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2887,7 +2887,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart79.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2969,11 +2969,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="57969521"/>
-        <c:axId val="93328663"/>
+        <c:axId val="43725350"/>
+        <c:axId val="64449001"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57969521"/>
+        <c:axId val="43725350"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2989,14 +2989,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93328663"/>
+        <c:crossAx val="64449001"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93328663"/>
+        <c:axId val="64449001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3021,7 +3021,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="57969521"/>
+        <c:crossAx val="43725350"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3056,7 +3056,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart80.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3150,11 +3150,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="42201669"/>
-        <c:axId val="89145638"/>
+        <c:axId val="82608297"/>
+        <c:axId val="1170742"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42201669"/>
+        <c:axId val="82608297"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3170,14 +3170,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89145638"/>
+        <c:crossAx val="1170742"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89145638"/>
+        <c:axId val="1170742"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3202,7 +3202,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="42201669"/>
+        <c:crossAx val="82608297"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3237,7 +3237,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart81.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3313,11 +3313,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="82537570"/>
-        <c:axId val="19842379"/>
+        <c:axId val="60792959"/>
+        <c:axId val="46405184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82537570"/>
+        <c:axId val="60792959"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3333,14 +3333,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19842379"/>
+        <c:crossAx val="46405184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19842379"/>
+        <c:axId val="46405184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3365,7 +3365,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82537570"/>
+        <c:crossAx val="60792959"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3400,7 +3400,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart82.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3464,11 +3464,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="46802690"/>
-        <c:axId val="47360332"/>
+        <c:axId val="85944030"/>
+        <c:axId val="67095593"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46802690"/>
+        <c:axId val="85944030"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3484,14 +3484,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47360332"/>
+        <c:crossAx val="67095593"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47360332"/>
+        <c:axId val="67095593"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3516,7 +3516,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="46802690"/>
+        <c:crossAx val="85944030"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3551,7 +3551,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart83.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3641,11 +3641,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="14397634"/>
-        <c:axId val="26864516"/>
+        <c:axId val="60503938"/>
+        <c:axId val="63134880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14397634"/>
+        <c:axId val="60503938"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3661,14 +3661,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="26864516"/>
+        <c:crossAx val="63134880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="26864516"/>
+        <c:axId val="63134880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3693,7 +3693,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14397634"/>
+        <c:crossAx val="60503938"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3728,7 +3728,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart84.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3812,11 +3812,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="96664211"/>
-        <c:axId val="9771586"/>
+        <c:axId val="44955864"/>
+        <c:axId val="24963501"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96664211"/>
+        <c:axId val="44955864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3832,14 +3832,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="9771586"/>
+        <c:crossAx val="24963501"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9771586"/>
+        <c:axId val="24963501"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3864,7 +3864,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96664211"/>
+        <c:crossAx val="44955864"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -3899,7 +3899,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart85.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4150,11 +4150,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="27991747"/>
-        <c:axId val="18838874"/>
+        <c:axId val="26035889"/>
+        <c:axId val="95607143"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="27991747"/>
+        <c:axId val="26035889"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4171,14 +4171,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="18838874"/>
+        <c:crossAx val="95607143"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18838874"/>
+        <c:axId val="95607143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4202,7 +4202,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27991747"/>
+        <c:crossAx val="26035889"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4238,7 +4238,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart86.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4358,11 +4358,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="92361597"/>
-        <c:axId val="3893469"/>
+        <c:axId val="62333310"/>
+        <c:axId val="27820112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92361597"/>
+        <c:axId val="62333310"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4379,14 +4379,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3893469"/>
+        <c:crossAx val="27820112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3893469"/>
+        <c:axId val="27820112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4412,7 +4412,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="92361597"/>
+        <c:crossAx val="62333310"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4438,7 +4438,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart87.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4720,11 +4720,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="70839024"/>
-        <c:axId val="37534261"/>
+        <c:axId val="97278312"/>
+        <c:axId val="99312559"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70839024"/>
+        <c:axId val="97278312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4741,14 +4741,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37534261"/>
+        <c:crossAx val="99312559"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37534261"/>
+        <c:axId val="99312559"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4772,7 +4772,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="70839024"/>
+        <c:crossAx val="97278312"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4798,7 +4798,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart88.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -4858,11 +4858,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="79965542"/>
-        <c:axId val="11569208"/>
+        <c:axId val="30937790"/>
+        <c:axId val="83258305"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79965542"/>
+        <c:axId val="30937790"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4879,14 +4879,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="11569208"/>
+        <c:crossAx val="83258305"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11569208"/>
+        <c:axId val="83258305"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4910,7 +4910,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79965542"/>
+        <c:crossAx val="30937790"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -4936,7 +4936,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart89.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5042,11 +5042,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="89118039"/>
-        <c:axId val="50983280"/>
+        <c:axId val="99452712"/>
+        <c:axId val="32144828"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="89118039"/>
+        <c:axId val="99452712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5063,14 +5063,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50983280"/>
+        <c:crossAx val="32144828"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50983280"/>
+        <c:axId val="32144828"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5095,7 +5095,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89118039"/>
+        <c:crossAx val="99452712"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -5121,7 +5121,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart70.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart90.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -5192,11 +5192,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="80580657"/>
-        <c:axId val="94971326"/>
+        <c:axId val="55728048"/>
+        <c:axId val="79659580"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80580657"/>
+        <c:axId val="55728048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5212,14 +5212,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="94971326"/>
+        <c:crossAx val="79659580"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94971326"/>
+        <c:axId val="79659580"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5244,7 +5244,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80580657"/>
+        <c:crossAx val="55728048"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -6336,8 +6336,8 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I30" activeCellId="0" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -6543,8 +6543,8 @@
   </sheetPr>
   <dimension ref="B1:K65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>

</xml_diff>

<commit_message>
avance concentrado de metricas
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
+++ b/Proyectos/2016/Métricas y monitoreo/Concentrado_Métricas_2016.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="129">
   <si>
     <t>Desviación de esfuerzo por proyectos planificados/reales</t>
   </si>
@@ -418,6 +418,9 @@
   <si>
     <t>Tickets de
 servicio</t>
+  </si>
+  <si>
+    <t>Contpaq i® Factura Electrónica U. Base Monoempresa Producto Nuevo Renta</t>
   </si>
 </sst>
 </file>
@@ -669,20 +672,20 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -892,7 +895,7 @@
                   <c:v>154239.88</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>154239.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1092,11 +1095,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="290343456"/>
-        <c:axId val="290345808"/>
+        <c:axId val="255540440"/>
+        <c:axId val="255541224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290343456"/>
+        <c:axId val="255540440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1117,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290345808"/>
+        <c:crossAx val="255541224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1122,7 +1125,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290345808"/>
+        <c:axId val="255541224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,7 +1150,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290343456"/>
+        <c:crossAx val="255540440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1269,7 +1272,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.91749999999999998</c:v>
+                  <c:v>0.93399999999999994</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1298,11 +1301,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292130768"/>
-        <c:axId val="292135080"/>
+        <c:axId val="257157104"/>
+        <c:axId val="257162200"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292130768"/>
+        <c:axId val="257157104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1319,7 +1322,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292135080"/>
+        <c:crossAx val="257162200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1327,7 +1330,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292135080"/>
+        <c:axId val="257162200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1353,7 +1356,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292130768"/>
+        <c:crossAx val="257157104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1522,11 +1525,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292136256"/>
-        <c:axId val="292137040"/>
+        <c:axId val="257155144"/>
+        <c:axId val="257155536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292136256"/>
+        <c:axId val="257155144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,7 +1546,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292137040"/>
+        <c:crossAx val="257155536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1551,7 +1554,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292137040"/>
+        <c:axId val="257155536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1577,7 +1580,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292136256"/>
+        <c:crossAx val="257155144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1730,7 +1733,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.96300000000000008</c:v>
+                  <c:v>0.97225000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1759,11 +1762,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292293216"/>
-        <c:axId val="292294392"/>
+        <c:axId val="255544360"/>
+        <c:axId val="255544752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292293216"/>
+        <c:axId val="255544360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1780,7 +1783,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292294392"/>
+        <c:crossAx val="255544752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1788,7 +1791,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292294392"/>
+        <c:axId val="255544752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1817,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292293216"/>
+        <c:crossAx val="255544360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1950,7 +1953,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00%">
-                  <c:v>0.82140000000000002</c:v>
+                  <c:v>0.8571200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -1982,11 +1985,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292293608"/>
-        <c:axId val="292295960"/>
+        <c:axId val="257586064"/>
+        <c:axId val="257588808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292293608"/>
+        <c:axId val="257586064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2003,7 +2006,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292295960"/>
+        <c:crossAx val="257588808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2011,7 +2014,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292295960"/>
+        <c:axId val="257588808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2037,7 +2040,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292293608"/>
+        <c:crossAx val="257586064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2194,11 +2197,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292296352"/>
-        <c:axId val="292295176"/>
+        <c:axId val="257590376"/>
+        <c:axId val="257590768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292296352"/>
+        <c:axId val="257590376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,7 +2218,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292295176"/>
+        <c:crossAx val="257590768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2223,7 +2226,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292295176"/>
+        <c:axId val="257590768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2249,7 +2252,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292296352"/>
+        <c:crossAx val="257590376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2415,7 +2418,7 @@
                   <c:v>275000.01</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>275000.01</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2583,11 +2586,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="292297136"/>
-        <c:axId val="292291256"/>
+        <c:axId val="257588024"/>
+        <c:axId val="257592728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292297136"/>
+        <c:axId val="257588024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2605,7 +2608,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292291256"/>
+        <c:crossAx val="257592728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2613,7 +2616,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292291256"/>
+        <c:axId val="257592728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2638,7 +2641,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292297136"/>
+        <c:crossAx val="257588024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2818,11 +2821,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="292297528"/>
-        <c:axId val="292292040"/>
+        <c:axId val="257592336"/>
+        <c:axId val="257586456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292297528"/>
+        <c:axId val="257592336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2840,7 +2843,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292292040"/>
+        <c:crossAx val="257586456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2848,7 +2851,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292292040"/>
+        <c:axId val="257586456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2875,7 +2878,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292297528"/>
+        <c:crossAx val="257592336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2961,123 +2964,27 @@
             <c:strRef>
               <c:f>Producto!$A$2:$A$40</c:f>
               <c:strCache>
-                <c:ptCount val="39"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Contpaq i® Nominas U. Base Renovación Renta</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Contpaq i® Factura Electrónica U. Base Monoempresa Renovación Renta</c:v>
+                  <c:v>Paquete de 2 horas de Asesoría y Soporte Técnico Contpaq i®, Servicio vía Remota (Incluye 2 horas gratis por ser cliente distinguido)</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Contpaq i® Factura Electrónica U. Base Multiempresa Renovación Renta</c:v>
+                  <c:v>Servicio de Asesoría y Soporte Técnico Vía Remota</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Paquete de 2 horas de Asesoría y Soporte Técnico Contpaq i®, Servicio vía Remota (Incluye 2 horas gratis por ser cliente distinguido)</c:v>
+                  <c:v>Contpaq i® CFDI en linea+ Producto Nuevo Monoempresa Renta</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Servicio de Asesoría y Soporte Técnico Vía Remota</c:v>
+                  <c:v>Contpaq i® Contabilidad U. Base Actualización Especial Tradicional</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Contpaq i® CFDI en linea+ Producto Nuevo Monoempresa Renta</c:v>
+                  <c:v>Paquete de 5 horas de Asesoría y Soporte Técnico Contpaq i®, Servicio vía Remota</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>Contpaq i® Contabilidad U. Base Actualización Especial Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Contpaq i® Comercial U. Base Renovación Renta</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Contpaq i® Contabilidad U. Base Actualización Normal Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Contpaq i® Nominas U. Base Actualización Especial Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Paquete de 5 horas de Asesoría y Soporte Técnico Contpaq i®, Servicio vía Remota</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Contpaq i® Comercial U. Base Producto Nuevo Renta</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Contpaq i® Contabilidad U. Adicional Producto Nuevo Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Contpaq i® Nominas U. Adicional Renovación Renta</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Contpaq i® Contabilidad U. Base Producto Nuevo Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>Paquete de 10 horas de Asesoría y Soporte Técnico Contpaq i®, Servicio vía Remota</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>Contpaq i® Bancos U. Base Actualización Especial Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>Servicio Presencial</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>Contpaq i® Contabilidad U. Adicional Actualización Especial Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>Contpaq i® Comercial U. Adicional Renovación Renta</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>Contpaq i® Bancos U. Base Producto Nuevo Renta</c:v>
-                </c:pt>
-                <c:pt idx="21">
                   <c:v>Contpaq i® Nominas U. Base Producto Nuevo Renta</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>Contpaq i® Nominas U. Adicional Actualización Especial Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>Contpaq i® Factura Electrónica U. Base Multiempresa Producto Nuevo Renta</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>Contpaq i® Factura Electrónica U. Base Actualización Especial Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Contpaq i® Comercial U. Adicional Producto Nuevo Renta</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Paquete de 500 timbres Contpaq i®</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Contpaq i® Factura Electrónica U. Adicional Multiempresa Renovación Renta</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Contpaq i® Contabilidad U. Adicional Producto Nuevo Renta</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Servicio por hora de Desarrollo Personalizado de JoinData</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Contpaq i® XML Línea + Multiempresa, Multiusuario Renta</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Contpaq i® Bancos U. Adicional Actualización Especial Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>XP/VS Terminal Server Lite Conexión a 1 servidor</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Contpaq i® CFDI Nóminas+ Producto Nuevo Monoempresa Renta</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Contpaq i® Nominas U. Adicional Producto Nuevo Tradicional</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Contpaq i® Factura Electrónica U. Adicional Monoempresa Renovación Renta</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Servicio de Implementación, Activación y Capacitación de CFDI Facturación en linea +</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Servicio de Asesoría y Soporte Contpaqi Contabilidad Vía Remota</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Cargo por gastos administrativos por cancelación de pedido</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3087,123 +2994,27 @@
               <c:f>Producto!$B$2:$B$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>83</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3233,11 +3044,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="292297920"/>
-        <c:axId val="292290472"/>
+        <c:axId val="257589592"/>
+        <c:axId val="257587632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292297920"/>
+        <c:axId val="257589592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3255,7 +3066,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292290472"/>
+        <c:crossAx val="257587632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3263,7 +3074,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292290472"/>
+        <c:axId val="257587632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3288,7 +3099,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292297920"/>
+        <c:crossAx val="257589592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3391,10 +3202,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3424,11 +3235,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="292292824"/>
-        <c:axId val="292294000"/>
+        <c:axId val="257591160"/>
+        <c:axId val="257591552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292292824"/>
+        <c:axId val="257591160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3446,7 +3257,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292294000"/>
+        <c:crossAx val="257591552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3454,7 +3265,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292294000"/>
+        <c:axId val="257591552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3479,7 +3290,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292292824"/>
+        <c:crossAx val="257591160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3579,7 +3390,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.48</c:v>
+                  <c:v>5.8823529411764705E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3702,11 +3513,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="293107312"/>
-        <c:axId val="293103784"/>
+        <c:axId val="257591944"/>
+        <c:axId val="257585672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="293107312"/>
+        <c:axId val="257591944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3723,7 +3534,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="293103784"/>
+        <c:crossAx val="257585672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3731,7 +3542,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="293103784"/>
+        <c:axId val="257585672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -3757,7 +3568,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="293107312"/>
+        <c:crossAx val="257591944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3902,7 +3713,7 @@
                   <c:v>-0.49686760648413364</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -3953,11 +3764,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="290347768"/>
-        <c:axId val="290346592"/>
+        <c:axId val="255541616"/>
+        <c:axId val="255547104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290347768"/>
+        <c:axId val="255541616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3975,7 +3786,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290346592"/>
+        <c:crossAx val="255547104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3983,7 +3794,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290346592"/>
+        <c:axId val="255547104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4008,7 +3819,7 @@
             <a:noFill/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290347768"/>
+        <c:crossAx val="255541616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4117,16 +3928,16 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.42499999999999999</c:v>
+                  <c:v>0.53333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.66664999999999996</c:v>
+                  <c:v>0.77776666666666661</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.72499999999999998</c:v>
+                  <c:v>0.56666666666666665</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4155,11 +3966,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="293104568"/>
-        <c:axId val="293104176"/>
+        <c:axId val="316050704"/>
+        <c:axId val="316048352"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="293104568"/>
+        <c:axId val="316050704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4176,7 +3987,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="293104176"/>
+        <c:crossAx val="316048352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4184,7 +3995,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="293104176"/>
+        <c:axId val="316048352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4210,7 +4021,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="293104568"/>
+        <c:crossAx val="316050704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4375,6 +4186,9 @@
                 <c:pt idx="3">
                   <c:v>80</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4500,6 +4314,9 @@
                 <c:pt idx="3">
                   <c:v>43</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>53</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4527,11 +4344,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="290342280"/>
-        <c:axId val="290343064"/>
+        <c:axId val="255542008"/>
+        <c:axId val="255546712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290342280"/>
+        <c:axId val="255542008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4548,7 +4365,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290343064"/>
+        <c:crossAx val="255546712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4556,7 +4373,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290343064"/>
+        <c:axId val="255546712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4582,7 +4399,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290342280"/>
+        <c:crossAx val="255542008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4747,6 +4564,9 @@
                 <c:pt idx="3">
                   <c:v>126</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>126</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4872,6 +4692,9 @@
                 <c:pt idx="3">
                   <c:v>121</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>144</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4899,11 +4722,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="290341888"/>
-        <c:axId val="290344632"/>
+        <c:axId val="255543968"/>
+        <c:axId val="255540048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290341888"/>
+        <c:axId val="255543968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4920,7 +4743,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290344632"/>
+        <c:crossAx val="255540048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4928,7 +4751,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="290344632"/>
+        <c:axId val="255540048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4954,7 +4777,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290341888"/>
+        <c:crossAx val="255543968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5120,7 +4943,7 @@
                   <c:v>-0.46250000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>-0.33750000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -5170,11 +4993,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="290345416"/>
-        <c:axId val="292136648"/>
+        <c:axId val="257157888"/>
+        <c:axId val="257161416"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="290345416"/>
+        <c:axId val="257157888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5191,7 +5014,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292136648"/>
+        <c:crossAx val="257161416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5199,7 +5022,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292136648"/>
+        <c:axId val="257161416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5225,7 +5048,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="290345416"/>
+        <c:crossAx val="257157888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5391,7 +5214,7 @@
                   <c:v>-3.9682539682539653E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.14285714285714279</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -5441,11 +5264,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292131552"/>
-        <c:axId val="292132336"/>
+        <c:axId val="257156712"/>
+        <c:axId val="257158672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292131552"/>
+        <c:axId val="257156712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5462,7 +5285,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292132336"/>
+        <c:crossAx val="257158672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5470,7 +5293,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292132336"/>
+        <c:axId val="257158672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5496,7 +5319,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292131552"/>
+        <c:crossAx val="257156712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5617,7 +5440,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.625</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5646,11 +5469,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292134688"/>
-        <c:axId val="292132728"/>
+        <c:axId val="257158280"/>
+        <c:axId val="257161808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292134688"/>
+        <c:axId val="257158280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5667,7 +5490,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292132728"/>
+        <c:crossAx val="257161808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5675,7 +5498,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292132728"/>
+        <c:axId val="257161808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5701,7 +5524,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292134688"/>
+        <c:crossAx val="257158280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5863,11 +5686,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292138216"/>
-        <c:axId val="292131944"/>
+        <c:axId val="257159848"/>
+        <c:axId val="257160240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292138216"/>
+        <c:axId val="257159848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5884,7 +5707,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292131944"/>
+        <c:crossAx val="257160240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5892,7 +5715,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292131944"/>
+        <c:axId val="257160240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5918,7 +5741,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292138216"/>
+        <c:crossAx val="257159848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6074,11 +5897,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="292135864"/>
-        <c:axId val="292133120"/>
+        <c:axId val="257155928"/>
+        <c:axId val="257160632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="292135864"/>
+        <c:axId val="257155928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6095,7 +5918,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292133120"/>
+        <c:crossAx val="257160632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6103,7 +5926,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="292133120"/>
+        <c:axId val="257160632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6129,7 +5952,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="292135864"/>
+        <c:crossAx val="257155928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7093,8 +6916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7115,65 +6938,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="4" spans="2:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="B4" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="45" t="s">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="45" t="s">
+      <c r="H4" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="45" t="s">
+      <c r="I4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="49" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="49"/>
-      <c r="C5" s="48" t="s">
+      <c r="B5" s="46"/>
+      <c r="C5" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48" t="s">
+      <c r="D5" s="47"/>
+      <c r="E5" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="48"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="49"/>
+      <c r="B6" s="46"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
@@ -7186,11 +7009,11 @@
       <c r="F6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
+      <c r="I6" s="48"/>
+      <c r="J6" s="45"/>
+      <c r="K6" s="45"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
@@ -7337,24 +7160,28 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="37"/>
+      <c r="C11" s="37">
+        <v>77119.94</v>
+      </c>
       <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="E11" s="37">
+        <v>77119.94</v>
+      </c>
       <c r="F11" s="37"/>
       <c r="G11" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>154239.88</v>
       </c>
       <c r="H11" s="12">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I11" s="11" t="e">
+      <c r="I11" s="11">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="J11" s="41"/>
       <c r="K11" s="40">
@@ -7546,16 +7373,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I4:I6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="K4:K6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
     <mergeCell ref="C1:G2"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:G6"/>
     <mergeCell ref="H4:H6"/>
-    <mergeCell ref="I4:I6"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="K4:K6"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -7568,7 +7395,7 @@
   <dimension ref="A2:C3"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7592,13 +7419,13 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="31">
         <f>B3/SUM(B3:C3)</f>
-        <v>0.48</v>
+        <v>5.8823529411764705E-2</v>
       </c>
       <c r="B3" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -7617,7 +7444,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7629,25 +7456,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="48" t="s">
+      <c r="A1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -7715,10 +7542,16 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="16"/>
+      <c r="B8" s="16">
+        <v>0.75</v>
+      </c>
       <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -7789,7 +7622,7 @@
       </c>
       <c r="B16" s="20">
         <f>AVERAGE(B4:B15)</f>
-        <v>0.42499999999999999</v>
+        <v>0.53333333333333333</v>
       </c>
       <c r="C16" s="19">
         <f>AVERAGE(C4:C15)</f>
@@ -7797,11 +7630,11 @@
       </c>
       <c r="D16" s="36">
         <f>AVERAGE(D4:D15)</f>
-        <v>0.66664999999999996</v>
+        <v>0.77776666666666661</v>
       </c>
       <c r="E16" s="19">
         <f>AVERAGE(E4:E15)</f>
-        <v>0.72499999999999998</v>
+        <v>0.56666666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -7823,8 +7656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J18"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7843,51 +7676,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="4" spans="2:10" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="B4" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="48"/>
-      <c r="C5" s="48" t="s">
+      <c r="B5" s="47"/>
+      <c r="C5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48" t="s">
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="48"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
@@ -8013,17 +7846,25 @@
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5" t="e">
+      <c r="C11" s="4">
+        <v>80</v>
+      </c>
+      <c r="D11" s="4">
+        <v>53</v>
+      </c>
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5" t="e">
+        <v>-0.33750000000000002</v>
+      </c>
+      <c r="F11" s="4">
+        <v>126</v>
+      </c>
+      <c r="G11" s="4">
+        <v>144</v>
+      </c>
+      <c r="H11" s="5">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.14285714285714279</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -8164,8 +8005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K50" sqref="K50"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8190,27 +8031,27 @@
       <c r="E3"/>
     </row>
     <row r="4" spans="3:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="48" t="s">
+      <c r="C4" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
     </row>
     <row r="6" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="48"/>
+      <c r="C6" s="47"/>
       <c r="D6" s="22" t="s">
         <v>46</v>
       </c>
@@ -8278,7 +8119,9 @@
       <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="16"/>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -8352,7 +8195,7 @@
       </c>
       <c r="D19" s="20">
         <f>AVERAGE(D7:D18)</f>
-        <v>0.625</v>
+        <v>0.7</v>
       </c>
       <c r="E19" s="19">
         <f>AVERAGE(E7:E18)</f>
@@ -8383,8 +8226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:H20"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8406,25 +8249,25 @@
       <c r="H1" s="25"/>
     </row>
     <row r="2" spans="3:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="45" t="s">
+      <c r="C2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="45"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="48"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="3:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="C4" s="48"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="22" t="s">
         <v>52</v>
       </c>
@@ -8483,7 +8326,9 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="15"/>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
     </row>
@@ -8549,7 +8394,7 @@
       </c>
       <c r="D17" s="19">
         <f>AVERAGE(D5:D16)</f>
-        <v>0.91749999999999998</v>
+        <v>0.93399999999999994</v>
       </c>
       <c r="E17" s="19">
         <f>AVERAGE(E5:E16)</f>
@@ -8577,8 +8422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView topLeftCell="A18" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8599,25 +8444,25 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="48" t="s">
+      <c r="C2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C4" s="48"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="1" t="s">
         <v>38</v>
       </c>
@@ -8811,29 +8656,29 @@
       <c r="D23"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="48" t="s">
+      <c r="C24" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="48"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="48"/>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
     </row>
     <row r="26" spans="3:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="C26" s="48"/>
+      <c r="C26" s="47"/>
       <c r="D26" s="7" t="s">
         <v>126</v>
       </c>
@@ -8911,7 +8756,9 @@
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
+      <c r="I30" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" s="2" t="s">
@@ -9027,7 +8874,7 @@
       </c>
       <c r="I39" s="19">
         <f t="shared" si="0"/>
-        <v>0.96300000000000008</v>
+        <v>0.97225000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -9047,8 +8894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:G38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9071,25 +8918,25 @@
       <c r="D1"/>
     </row>
     <row r="2" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="48" t="s">
+      <c r="C2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
     </row>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="48"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="14" t="s">
         <v>28</v>
       </c>
@@ -9175,10 +9022,18 @@
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+      <c r="G9" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C10" s="2" t="s">
@@ -9257,7 +9112,7 @@
       </c>
       <c r="F17" s="16">
         <f>AVERAGE(F5:F16)</f>
-        <v>0.82140000000000002</v>
+        <v>0.8571200000000001</v>
       </c>
       <c r="G17" s="15">
         <f>AVERAGE(G5:G16)</f>
@@ -9280,25 +9135,25 @@
       <c r="D22"/>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D23" s="48" t="s">
+      <c r="C23" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="48"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
     </row>
     <row r="25" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C25" s="48"/>
+      <c r="C25" s="47"/>
       <c r="D25" s="1" t="s">
         <v>33</v>
       </c>
@@ -9466,8 +9321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9488,55 +9343,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="48" t="s">
+      <c r="A1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="45" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="45" t="s">
+      <c r="I1" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="47" t="s">
+      <c r="L1" s="45" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48" t="s">
+      <c r="C2" s="47"/>
+      <c r="D2" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48" t="s">
+      <c r="E2" s="47"/>
+      <c r="F2" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="45"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="1" t="s">
         <v>63</v>
       </c>
@@ -9555,11 +9410,11 @@
       <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="47"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="45"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -9735,24 +9590,36 @@
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="B8" s="10">
+        <v>91666.67</v>
+      </c>
+      <c r="C8" s="10">
+        <v>44102</v>
+      </c>
+      <c r="D8" s="10">
+        <v>91666.67</v>
+      </c>
+      <c r="E8" s="10">
+        <v>62184</v>
+      </c>
+      <c r="F8" s="10">
+        <v>91666.67</v>
+      </c>
+      <c r="G8" s="10">
+        <v>27020</v>
+      </c>
       <c r="H8" s="26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>275000.01</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>133306</v>
       </c>
       <c r="J8" s="27"/>
-      <c r="K8" s="29" t="e">
+      <c r="K8" s="29">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>-100</v>
       </c>
       <c r="L8" s="9">
         <f>J8-'Desviacion de costos'!K11</f>
@@ -9961,35 +9828,35 @@
       </c>
       <c r="B16" s="10">
         <f t="shared" ref="B16:J16" si="3">SUM(B4:B15)</f>
-        <v>275000.01</v>
+        <v>366666.68</v>
       </c>
       <c r="C16" s="10">
         <f t="shared" si="3"/>
-        <v>77307</v>
+        <v>121409</v>
       </c>
       <c r="D16" s="10">
         <f t="shared" si="3"/>
-        <v>412500.00999999995</v>
+        <v>504166.67999999993</v>
       </c>
       <c r="E16" s="10">
         <f t="shared" si="3"/>
-        <v>144691.51</v>
+        <v>206875.51</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="3"/>
-        <v>412500.00999999995</v>
+        <v>504166.67999999993</v>
       </c>
       <c r="G16" s="10">
         <f t="shared" si="3"/>
-        <v>123988.93</v>
+        <v>151008.93</v>
       </c>
       <c r="H16" s="26">
         <f t="shared" si="3"/>
-        <v>1100000.03</v>
+        <v>1375000.04</v>
       </c>
       <c r="I16" s="10">
         <f t="shared" si="3"/>
-        <v>345987.44</v>
+        <v>479293.44</v>
       </c>
       <c r="J16" s="27">
         <f t="shared" si="3"/>
@@ -9997,7 +9864,7 @@
       </c>
       <c r="K16" s="29">
         <f t="shared" si="2"/>
-        <v>-48.249715047735044</v>
+        <v>-58.599772113461178</v>
       </c>
       <c r="L16" s="9">
         <f>J16-'Desviacion de costos'!K19</f>
@@ -10005,14 +9872,14 @@
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="47"/>
+      <c r="C18" s="45"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="47"/>
-      <c r="C19" s="47"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="30" t="s">
@@ -10042,17 +9909,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="J1:J3"/>
     <mergeCell ref="B18:C19"/>
     <mergeCell ref="K1:K3"/>
     <mergeCell ref="L1:L3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="J1:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -10065,7 +9932,7 @@
   <dimension ref="C2:D17"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10078,20 +9945,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="48" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="45" t="s">
+      <c r="C2" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="48" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="48"/>
-      <c r="D4" s="45"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
@@ -10197,8 +10064,8 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10260,7 +10127,7 @@
       </c>
       <c r="B2" s="33">
         <f t="shared" ref="B2:B40" si="0">SUM(C2:N2)</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C2" s="34">
         <v>10</v>
@@ -10274,7 +10141,9 @@
       <c r="F2" s="3">
         <v>9</v>
       </c>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3">
+        <v>10</v>
+      </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -10283,7 +10152,7 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>73</v>
       </c>
@@ -10308,7 +10177,7 @@
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
     </row>
-    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>74</v>
       </c>
@@ -10343,7 +10212,7 @@
       </c>
       <c r="B5" s="33">
         <f t="shared" si="0"/>
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C5" s="34">
         <v>12</v>
@@ -10357,7 +10226,9 @@
       <c r="F5" s="3">
         <v>17</v>
       </c>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>20</v>
+      </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -10372,7 +10243,7 @@
       </c>
       <c r="B6" s="33">
         <f t="shared" si="0"/>
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C6" s="34">
         <v>33</v>
@@ -10386,7 +10257,9 @@
       <c r="F6" s="3">
         <v>9</v>
       </c>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>10</v>
+      </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -10401,7 +10274,7 @@
       </c>
       <c r="B7" s="33">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C7" s="34">
         <v>4</v>
@@ -10415,7 +10288,9 @@
       <c r="F7" s="3">
         <v>7</v>
       </c>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3">
+        <v>9</v>
+      </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -10430,7 +10305,7 @@
       </c>
       <c r="B8" s="33">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" s="34">
         <v>6</v>
@@ -10444,7 +10319,9 @@
       <c r="F8" s="3">
         <v>3</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -10453,7 +10330,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33" t="s">
         <v>79</v>
       </c>
@@ -10476,7 +10353,7 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33" t="s">
         <v>80</v>
       </c>
@@ -10501,7 +10378,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33" t="s">
         <v>81</v>
       </c>
@@ -10532,7 +10409,7 @@
       </c>
       <c r="B12" s="33">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C12" s="34">
         <v>2</v>
@@ -10546,7 +10423,9 @@
       <c r="F12" s="3">
         <v>3</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="3">
+        <v>4</v>
+      </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -10555,7 +10434,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
         <v>83</v>
       </c>
@@ -10578,7 +10457,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
         <v>84</v>
       </c>
@@ -10605,7 +10484,7 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33" t="s">
         <v>85</v>
       </c>
@@ -10632,7 +10511,7 @@
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33" t="s">
         <v>86</v>
       </c>
@@ -10657,7 +10536,7 @@
       <c r="M16" s="3"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>87</v>
       </c>
@@ -10680,7 +10559,7 @@
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>88</v>
       </c>
@@ -10705,7 +10584,7 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
         <v>89</v>
       </c>
@@ -10732,7 +10611,7 @@
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
         <v>90</v>
       </c>
@@ -10757,7 +10636,7 @@
       <c r="M20" s="3"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>91</v>
       </c>
@@ -10780,7 +10659,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>92</v>
       </c>
@@ -10809,13 +10688,15 @@
       </c>
       <c r="B23" s="33">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="34"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="G23" s="3">
+        <v>5</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
@@ -10824,7 +10705,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33" t="s">
         <v>94</v>
       </c>
@@ -10847,7 +10728,7 @@
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>95</v>
       </c>
@@ -10872,7 +10753,7 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33" t="s">
         <v>96</v>
       </c>
@@ -10895,7 +10776,7 @@
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
         <v>97</v>
       </c>
@@ -10918,7 +10799,7 @@
       <c r="M27" s="3"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
         <v>98</v>
       </c>
@@ -10941,7 +10822,7 @@
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>99</v>
       </c>
@@ -10964,7 +10845,7 @@
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
         <v>100</v>
       </c>
@@ -10987,7 +10868,7 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
         <v>101</v>
       </c>
@@ -11014,7 +10895,7 @@
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="33" t="s">
         <v>102</v>
       </c>
@@ -11037,7 +10918,7 @@
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>103</v>
       </c>
@@ -11062,7 +10943,7 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="33" t="s">
         <v>104</v>
       </c>
@@ -11085,7 +10966,7 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>105</v>
       </c>
@@ -11110,7 +10991,7 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
     </row>
-    <row r="36" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
         <v>106</v>
       </c>
@@ -11131,7 +11012,7 @@
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
     </row>
-    <row r="37" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
         <v>107</v>
       </c>
@@ -11156,7 +11037,7 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
     </row>
-    <row r="38" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
         <v>108</v>
       </c>
@@ -11179,7 +11060,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
     </row>
-    <row r="39" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
         <v>109</v>
       </c>
@@ -11202,7 +11083,7 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
     </row>
-    <row r="40" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="33" t="s">
         <v>110</v>
       </c>
@@ -11224,7 +11105,7 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
     </row>
-    <row r="41" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="33" t="s">
         <v>111</v>
       </c>
@@ -11255,7 +11136,9 @@
       <c r="F42" s="34">
         <v>3</v>
       </c>
-      <c r="G42" s="34"/>
+      <c r="G42" s="34">
+        <v>4</v>
+      </c>
       <c r="H42" s="34"/>
       <c r="I42" s="34"/>
       <c r="J42" s="34"/>
@@ -11264,7 +11147,7 @@
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
     </row>
-    <row r="43" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="33" t="s">
         <v>121</v>
       </c>
@@ -11284,8 +11167,25 @@
       <c r="M43" s="34"/>
       <c r="N43" s="34"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="35"/>
+    <row r="44" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34">
+        <v>3</v>
+      </c>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="34"/>
+      <c r="N44" s="34"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="35"/>

</xml_diff>